<commit_message>
Added output Field. Improved Error Reporting on Clone. Trying out new data
</commit_message>
<xml_diff>
--- a/supplementary/Expanded Reproduction/Expanded Reproduction Only.xlsx
+++ b/supplementary/Expanded Reproduction/Expanded Reproduction Only.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\Documents\My Works\REPOS\simulation-api\supplementary\Expanded Reproduction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4197F320-6AD7-4109-B37B-555BA85B9807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9CB03D-169E-4BEA-A60D-798CED2F3EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1286" yWindow="1011" windowWidth="8931" windowHeight="9635" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Marx 1" sheetId="4" r:id="rId1"/>
@@ -1085,7 +1085,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1093,7 +1093,7 @@
     <col min="3" max="3" width="9.07421875" customWidth="1"/>
     <col min="4" max="4" width="6.765625" customWidth="1"/>
     <col min="5" max="5" width="7.4609375" customWidth="1"/>
-    <col min="6" max="6" width="7.23046875" customWidth="1"/>
+    <col min="6" max="6" width="7.61328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.3828125" customWidth="1"/>
     <col min="8" max="8" width="6.69140625" customWidth="1"/>
     <col min="9" max="9" width="6.23046875" customWidth="1"/>

</xml_diff>